<commit_message>
Updated plot data to fix data entry error that assigned trees from plot 41 to plot 56.
</commit_message>
<xml_diff>
--- a/Data/RawData/YPE_Data/YPE_41/Digital Data_YPE41/YPE_Treedata_Plot_41.xlsx
+++ b/Data/RawData/YPE_Data/YPE_41/Digital Data_YPE41/YPE_Treedata_Plot_41.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifercribbs/Documents/YOSE/Analysis/MultipleDisturbances/Data/RawData/YPE_Data/YPE_41/Digital Data_YPE41/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7346E4-4F09-D641-93BD-7C1C4439700F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="r6qEI0wk47A0SlgJKRUw+LbCmlZiTJdNi+CE0CuWnr4="/>
@@ -234,25 +243,28 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -261,45 +273,46 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -489,23 +502,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="6" width="12.63"/>
+    <col min="1" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,21 +567,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>16</v>
@@ -584,7 +602,7 @@
         <v>12.2</v>
       </c>
       <c r="L2" s="2">
-        <v>97.0</v>
+        <v>97</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>14</v>
@@ -593,21 +611,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>16</v>
@@ -628,7 +646,7 @@
         <v>2.8</v>
       </c>
       <c r="L3" s="2">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>18</v>
@@ -637,21 +655,21 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>20</v>
@@ -672,7 +690,7 @@
         <v>9.1</v>
       </c>
       <c r="L4" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>14</v>
@@ -681,21 +699,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>21</v>
@@ -707,7 +725,7 @@
         <v>14</v>
       </c>
       <c r="I5" s="2">
-        <v>-1.1</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="J5" s="2">
         <v>39.4</v>
@@ -716,7 +734,7 @@
         <v>18.7</v>
       </c>
       <c r="L5" s="2">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>14</v>
@@ -725,30 +743,30 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="2">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H6" s="2">
-        <v>1.09</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>14</v>
@@ -757,10 +775,10 @@
         <v>7.5</v>
       </c>
       <c r="K6" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L6" s="2">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>14</v>
@@ -769,21 +787,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>20</v>
@@ -804,7 +822,7 @@
         <v>4.12</v>
       </c>
       <c r="L7" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>14</v>
@@ -813,21 +831,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>20</v>
@@ -848,7 +866,7 @@
         <v>15.5</v>
       </c>
       <c r="L8" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>14</v>
@@ -857,21 +875,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>24</v>
@@ -889,10 +907,10 @@
         <v>31.5</v>
       </c>
       <c r="K9" s="2">
-        <v>8.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="L9" s="2">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>18</v>
@@ -901,21 +919,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>26</v>
@@ -933,10 +951,10 @@
         <v>13.1</v>
       </c>
       <c r="K10" s="2">
-        <v>8.3</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="L10" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>14</v>
@@ -945,27 +963,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G11" s="2">
-        <v>8.8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="H11" s="2">
         <v>4.7</v>
@@ -980,7 +998,7 @@
         <v>24.8</v>
       </c>
       <c r="L11" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>14</v>
@@ -989,27 +1007,27 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="2">
-        <v>18.4</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>14</v>
@@ -1024,7 +1042,7 @@
         <v>1.7</v>
       </c>
       <c r="L12" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>14</v>
@@ -1033,27 +1051,27 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G13" s="2">
-        <v>18.4</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="H13" s="2">
         <v>3.7</v>
@@ -1068,7 +1086,7 @@
         <v>14.5</v>
       </c>
       <c r="L13" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>14</v>
@@ -1077,21 +1095,21 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>20</v>
@@ -1106,13 +1124,13 @@
         <v>14</v>
       </c>
       <c r="J14" s="2">
-        <v>16.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="K14" s="2">
         <v>7.6</v>
       </c>
       <c r="L14" s="2">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>14</v>
@@ -1121,21 +1139,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>16</v>
@@ -1156,7 +1174,7 @@
         <v>2.1</v>
       </c>
       <c r="L15" s="2">
-        <v>96.0</v>
+        <v>96</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>32</v>
@@ -1165,21 +1183,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>16</v>
@@ -1200,7 +1218,7 @@
         <v>4.5</v>
       </c>
       <c r="L16" s="2">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>14</v>
@@ -1209,21 +1227,21 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>16</v>
@@ -1244,7 +1262,7 @@
         <v>2.9</v>
       </c>
       <c r="L17" s="2">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>14</v>
@@ -1253,21 +1271,21 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>16</v>
@@ -1288,7 +1306,7 @@
         <v>1.25</v>
       </c>
       <c r="L18" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>14</v>
@@ -1297,21 +1315,21 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>20</v>
@@ -1329,10 +1347,10 @@
         <v>8.4</v>
       </c>
       <c r="K19" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="L19" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>14</v>
@@ -1341,42 +1359,42 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G20" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="H20" s="2">
-        <v>2.45</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J20" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K20" s="2">
         <v>1.35</v>
       </c>
       <c r="L20" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>14</v>
@@ -1385,21 +1403,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>16</v>
@@ -1420,7 +1438,7 @@
         <v>2.1</v>
       </c>
       <c r="L21" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>14</v>
@@ -1429,21 +1447,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E22" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>16</v>
@@ -1464,7 +1482,7 @@
         <v>2.6</v>
       </c>
       <c r="L22" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>14</v>
@@ -1473,21 +1491,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>20</v>
@@ -1502,13 +1520,13 @@
         <v>14</v>
       </c>
       <c r="J23" s="2">
-        <v>72.1</v>
+        <v>72.099999999999994</v>
       </c>
       <c r="K23" s="2">
         <v>15.3</v>
       </c>
       <c r="L23" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>40</v>
@@ -1517,21 +1535,21 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E24" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>16</v>
@@ -1552,7 +1570,7 @@
         <v>6.4</v>
       </c>
       <c r="L24" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>14</v>
@@ -1561,21 +1579,21 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E25" s="2">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>20</v>
@@ -1590,13 +1608,13 @@
         <v>14</v>
       </c>
       <c r="J25" s="2">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="K25" s="2">
         <v>3.9</v>
       </c>
       <c r="L25" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>18</v>
@@ -1605,21 +1623,21 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E26" s="2">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>20</v>
@@ -1640,7 +1658,7 @@
         <v>3.2</v>
       </c>
       <c r="L26" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>18</v>
@@ -1649,21 +1667,21 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E27" s="2">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>16</v>
@@ -1678,13 +1696,13 @@
         <v>45</v>
       </c>
       <c r="J27" s="2">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="K27" s="2">
         <v>3.4</v>
       </c>
       <c r="L27" s="2">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>14</v>
@@ -1693,21 +1711,21 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E28" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>20</v>
@@ -1722,13 +1740,13 @@
         <v>-1.86</v>
       </c>
       <c r="J28" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="K28" s="2">
         <v>5.8</v>
       </c>
       <c r="L28" s="2">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>14</v>
@@ -1737,21 +1755,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E29" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>20</v>
@@ -1769,10 +1787,10 @@
         <v>29.2</v>
       </c>
       <c r="K29" s="2">
-        <v>17.6</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="L29" s="2">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>14</v>
@@ -1781,21 +1799,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E30" s="2">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>21</v>
@@ -1810,13 +1828,13 @@
         <v>-0.46</v>
       </c>
       <c r="J30" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K30" s="2">
         <v>1.34</v>
       </c>
       <c r="L30" s="2">
-        <v>95.0</v>
+        <v>95</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>14</v>
@@ -1825,21 +1843,21 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E31" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>21</v>
@@ -1860,7 +1878,7 @@
         <v>1.9</v>
       </c>
       <c r="L31" s="2">
-        <v>93.0</v>
+        <v>93</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>14</v>
@@ -1869,27 +1887,27 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E32" s="2">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G32" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>14</v>
@@ -1901,10 +1919,10 @@
         <v>0.6</v>
       </c>
       <c r="K32" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="L32" s="2">
-        <v>97.0</v>
+        <v>97</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>14</v>
@@ -1913,21 +1931,21 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E33" s="2">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>21</v>
@@ -1942,13 +1960,13 @@
         <v>-1.26</v>
       </c>
       <c r="J33" s="2">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="K33" s="2">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="L33" s="2">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>14</v>
@@ -1957,21 +1975,21 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C34" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E34" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>21</v>
@@ -1980,7 +1998,7 @@
         <v>27.8</v>
       </c>
       <c r="H34" s="2">
-        <v>2.01</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>14</v>
@@ -1992,7 +2010,7 @@
         <v>2.15</v>
       </c>
       <c r="L34" s="2">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>14</v>
@@ -2001,21 +2019,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C35" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E35" s="2">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>16</v>
@@ -2030,13 +2048,13 @@
         <v>14</v>
       </c>
       <c r="J35" s="2">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="K35" s="2">
         <v>2.4</v>
       </c>
       <c r="L35" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>14</v>
@@ -2045,21 +2063,21 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C36" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E36" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>16</v>
@@ -2080,7 +2098,7 @@
         <v>2.6</v>
       </c>
       <c r="L36" s="2">
-        <v>97.0</v>
+        <v>97</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>14</v>
@@ -2089,21 +2107,21 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C37" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E37" s="2">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>26</v>
@@ -2112,7 +2130,7 @@
         <v>29.2</v>
       </c>
       <c r="H37" s="2">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>14</v>
@@ -2124,7 +2142,7 @@
         <v>2.4</v>
       </c>
       <c r="L37" s="2">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="M37" s="2" t="s">
         <v>14</v>
@@ -2133,21 +2151,21 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E38" s="2">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>16</v>
@@ -2168,7 +2186,7 @@
         <v>3.2</v>
       </c>
       <c r="L38" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>14</v>
@@ -2177,21 +2195,21 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C39" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E39" s="2">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>16</v>
@@ -2206,13 +2224,13 @@
         <v>14</v>
       </c>
       <c r="J39" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K39" s="2">
         <v>1.22</v>
       </c>
       <c r="L39" s="2">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>14</v>
@@ -2221,21 +2239,21 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C40" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E40" s="2">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>16</v>
@@ -2250,13 +2268,13 @@
         <v>14</v>
       </c>
       <c r="J40" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K40" s="2">
         <v>1.19</v>
       </c>
       <c r="L40" s="2">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>14</v>
@@ -2265,21 +2283,21 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C41" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E41" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>16</v>
@@ -2300,7 +2318,7 @@
         <v>6.8</v>
       </c>
       <c r="L41" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>14</v>
@@ -2309,21 +2327,21 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C42" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E42" s="2">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>21</v>
@@ -2341,10 +2359,10 @@
         <v>3.2</v>
       </c>
       <c r="K42" s="2">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="L42" s="2">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>14</v>
@@ -2353,21 +2371,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C43" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E43" s="2">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>21</v>
@@ -2382,13 +2400,13 @@
         <v>-0.69</v>
       </c>
       <c r="J43" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K43" s="2">
         <v>1.3</v>
       </c>
       <c r="L43" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>14</v>
@@ -2397,27 +2415,27 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C44" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E44" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G44" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>14</v>
@@ -2432,7 +2450,7 @@
         <v>24.3</v>
       </c>
       <c r="L44" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M44" s="2" t="s">
         <v>14</v>
@@ -2441,21 +2459,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
+    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C45" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E45" s="2">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>16</v>
@@ -2476,7 +2494,7 @@
         <v>6.1</v>
       </c>
       <c r="L45" s="2">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="M45" s="2" t="s">
         <v>14</v>
@@ -2485,42 +2503,42 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
+    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C46" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E46" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G46" s="2">
-        <v>35.3</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="H46" s="2">
-        <v>2.26</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J46" s="2">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="K46" s="2">
         <v>4.3</v>
       </c>
       <c r="L46" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M46" s="2" t="s">
         <v>14</v>
@@ -2529,27 +2547,27 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
+    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C47" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E47" s="2">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G47" s="2">
-        <v>35.7</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="H47" s="2">
         <v>0.94</v>
@@ -2561,10 +2579,10 @@
         <v>22.4</v>
       </c>
       <c r="K47" s="2">
-        <v>9.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="L47" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M47" s="2" t="s">
         <v>14</v>
@@ -2573,30 +2591,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C48" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E48" s="2">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G48" s="2">
-        <v>35.84</v>
+        <v>35.840000000000003</v>
       </c>
       <c r="H48" s="2">
-        <v>2.55</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>14</v>
@@ -2605,10 +2623,10 @@
         <v>7.4</v>
       </c>
       <c r="K48" s="2">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="L48" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="M48" s="2" t="s">
         <v>14</v>
@@ -2617,21 +2635,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
+    <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C49" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E49" s="2">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>20</v>
@@ -2649,10 +2667,10 @@
         <v>16.2</v>
       </c>
       <c r="K49" s="2">
-        <v>9.7</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="L49" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M49" s="2" t="s">
         <v>58</v>
@@ -2661,30 +2679,30 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
+    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C50" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E50" s="2">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G50" s="2">
-        <v>36.16</v>
+        <v>36.159999999999997</v>
       </c>
       <c r="H50" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>14</v>
@@ -2696,7 +2714,7 @@
         <v>3.4</v>
       </c>
       <c r="L50" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="M50" s="2" t="s">
         <v>14</v>
@@ -2705,21 +2723,21 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C51" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E51" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>21</v>
@@ -2731,7 +2749,7 @@
         <v>14</v>
       </c>
       <c r="I51" s="2">
-        <v>-1.13</v>
+        <v>-1.1299999999999999</v>
       </c>
       <c r="J51" s="2">
         <v>114.4</v>
@@ -2740,7 +2758,7 @@
         <v>32.9</v>
       </c>
       <c r="L51" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M51" s="2" t="s">
         <v>40</v>
@@ -2749,21 +2767,21 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C52" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E52" s="2">
-        <v>51.0</v>
+        <v>51</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>20</v>
@@ -2784,7 +2802,7 @@
         <v>13.7</v>
       </c>
       <c r="L52" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M52" s="2" t="s">
         <v>40</v>
@@ -2793,21 +2811,21 @@
         <v>62</v>
       </c>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
+    <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C53" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E53" s="2">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>20</v>
@@ -2828,7 +2846,7 @@
         <v>3.9</v>
       </c>
       <c r="L53" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M53" s="2" t="s">
         <v>40</v>
@@ -2837,21 +2855,21 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
+    <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C54" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E54" s="2">
-        <v>53.0</v>
+        <v>53</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>21</v>
@@ -2872,7 +2890,7 @@
         <v>1.4</v>
       </c>
       <c r="L54" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M54" s="2" t="s">
         <v>14</v>
@@ -2881,21 +2899,21 @@
         <v>63</v>
       </c>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
+    <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C55" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E55" s="2">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>20</v>
@@ -2916,7 +2934,7 @@
         <v>38.1</v>
       </c>
       <c r="L55" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M55" s="2" t="s">
         <v>14</v>
@@ -2925,21 +2943,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
+    <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C56" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E56" s="2">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>26</v>
@@ -2954,13 +2972,13 @@
         <v>-0.4</v>
       </c>
       <c r="J56" s="2">
-        <v>18.6</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="K56" s="2">
         <v>10.3</v>
       </c>
       <c r="L56" s="2">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="M56" s="2" t="s">
         <v>64</v>
@@ -2969,21 +2987,21 @@
         <v>65</v>
       </c>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
+    <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C57" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E57" s="2">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>16</v>
@@ -2998,13 +3016,13 @@
         <v>-0.45</v>
       </c>
       <c r="J57" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K57" s="2">
         <v>1.33</v>
       </c>
       <c r="L57" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M57" s="2" t="s">
         <v>14</v>
@@ -3013,21 +3031,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
+    <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C58" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E58" s="2">
-        <v>57.0</v>
+        <v>57</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>16</v>
@@ -3048,7 +3066,7 @@
         <v>4.8</v>
       </c>
       <c r="L58" s="2">
-        <v>97.0</v>
+        <v>97</v>
       </c>
       <c r="M58" s="2" t="s">
         <v>14</v>
@@ -3057,21 +3075,21 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
+    <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C59" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E59" s="2">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>16</v>
@@ -3080,7 +3098,7 @@
         <v>44.2</v>
       </c>
       <c r="H59" s="2">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>14</v>
@@ -3092,7 +3110,7 @@
         <v>2.8</v>
       </c>
       <c r="L59" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M59" s="2" t="s">
         <v>67</v>
@@ -3101,21 +3119,21 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
+    <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C60" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E60" s="2">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>26</v>
@@ -3136,7 +3154,7 @@
         <v>1.75</v>
       </c>
       <c r="L60" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="M60" s="2" t="s">
         <v>14</v>
@@ -3145,21 +3163,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
+    <row r="61" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C61" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E61" s="2">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>16</v>
@@ -3180,7 +3198,7 @@
         <v>4.7</v>
       </c>
       <c r="L61" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M61" s="2" t="s">
         <v>14</v>
@@ -3189,21 +3207,21 @@
         <v>69</v>
       </c>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C62" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E62" s="2">
-        <v>61.0</v>
+        <v>61</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>21</v>
@@ -3215,16 +3233,16 @@
         <v>14</v>
       </c>
       <c r="I62" s="2">
-        <v>-2.05</v>
+        <v>-2.0499999999999998</v>
       </c>
       <c r="J62" s="2">
         <v>22.8</v>
       </c>
       <c r="K62" s="2">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="L62" s="2">
-        <v>85.0</v>
+        <v>85</v>
       </c>
       <c r="M62" s="2" t="s">
         <v>14</v>
@@ -3233,21 +3251,21 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
+    <row r="63" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="2">
-        <v>56.0</v>
+        <v>41</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C63" s="3">
-        <v>45155.0</v>
+        <v>45155</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E63" s="2">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>26</v>
@@ -3265,10 +3283,10 @@
         <v>7.1</v>
       </c>
       <c r="K63" s="2">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="L63" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="M63" s="2" t="s">
         <v>14</v>
@@ -3277,944 +3295,944 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
-    <row r="115" ht="15.75" customHeight="1"/>
-    <row r="116" ht="15.75" customHeight="1"/>
-    <row r="117" ht="15.75" customHeight="1"/>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
-    <row r="149" ht="15.75" customHeight="1"/>
-    <row r="150" ht="15.75" customHeight="1"/>
-    <row r="151" ht="15.75" customHeight="1"/>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
-    <row r="161" ht="15.75" customHeight="1"/>
-    <row r="162" ht="15.75" customHeight="1"/>
-    <row r="163" ht="15.75" customHeight="1"/>
-    <row r="164" ht="15.75" customHeight="1"/>
-    <row r="165" ht="15.75" customHeight="1"/>
-    <row r="166" ht="15.75" customHeight="1"/>
-    <row r="167" ht="15.75" customHeight="1"/>
-    <row r="168" ht="15.75" customHeight="1"/>
-    <row r="169" ht="15.75" customHeight="1"/>
-    <row r="170" ht="15.75" customHeight="1"/>
-    <row r="171" ht="15.75" customHeight="1"/>
-    <row r="172" ht="15.75" customHeight="1"/>
-    <row r="173" ht="15.75" customHeight="1"/>
-    <row r="174" ht="15.75" customHeight="1"/>
-    <row r="175" ht="15.75" customHeight="1"/>
-    <row r="176" ht="15.75" customHeight="1"/>
-    <row r="177" ht="15.75" customHeight="1"/>
-    <row r="178" ht="15.75" customHeight="1"/>
-    <row r="179" ht="15.75" customHeight="1"/>
-    <row r="180" ht="15.75" customHeight="1"/>
-    <row r="181" ht="15.75" customHeight="1"/>
-    <row r="182" ht="15.75" customHeight="1"/>
-    <row r="183" ht="15.75" customHeight="1"/>
-    <row r="184" ht="15.75" customHeight="1"/>
-    <row r="185" ht="15.75" customHeight="1"/>
-    <row r="186" ht="15.75" customHeight="1"/>
-    <row r="187" ht="15.75" customHeight="1"/>
-    <row r="188" ht="15.75" customHeight="1"/>
-    <row r="189" ht="15.75" customHeight="1"/>
-    <row r="190" ht="15.75" customHeight="1"/>
-    <row r="191" ht="15.75" customHeight="1"/>
-    <row r="192" ht="15.75" customHeight="1"/>
-    <row r="193" ht="15.75" customHeight="1"/>
-    <row r="194" ht="15.75" customHeight="1"/>
-    <row r="195" ht="15.75" customHeight="1"/>
-    <row r="196" ht="15.75" customHeight="1"/>
-    <row r="197" ht="15.75" customHeight="1"/>
-    <row r="198" ht="15.75" customHeight="1"/>
-    <row r="199" ht="15.75" customHeight="1"/>
-    <row r="200" ht="15.75" customHeight="1"/>
-    <row r="201" ht="15.75" customHeight="1"/>
-    <row r="202" ht="15.75" customHeight="1"/>
-    <row r="203" ht="15.75" customHeight="1"/>
-    <row r="204" ht="15.75" customHeight="1"/>
-    <row r="205" ht="15.75" customHeight="1"/>
-    <row r="206" ht="15.75" customHeight="1"/>
-    <row r="207" ht="15.75" customHeight="1"/>
-    <row r="208" ht="15.75" customHeight="1"/>
-    <row r="209" ht="15.75" customHeight="1"/>
-    <row r="210" ht="15.75" customHeight="1"/>
-    <row r="211" ht="15.75" customHeight="1"/>
-    <row r="212" ht="15.75" customHeight="1"/>
-    <row r="213" ht="15.75" customHeight="1"/>
-    <row r="214" ht="15.75" customHeight="1"/>
-    <row r="215" ht="15.75" customHeight="1"/>
-    <row r="216" ht="15.75" customHeight="1"/>
-    <row r="217" ht="15.75" customHeight="1"/>
-    <row r="218" ht="15.75" customHeight="1"/>
-    <row r="219" ht="15.75" customHeight="1"/>
-    <row r="220" ht="15.75" customHeight="1"/>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
-    <row r="226" ht="15.75" customHeight="1"/>
-    <row r="227" ht="15.75" customHeight="1"/>
-    <row r="228" ht="15.75" customHeight="1"/>
-    <row r="229" ht="15.75" customHeight="1"/>
-    <row r="230" ht="15.75" customHeight="1"/>
-    <row r="231" ht="15.75" customHeight="1"/>
-    <row r="232" ht="15.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
-    <row r="234" ht="15.75" customHeight="1"/>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
-    <row r="238" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
-    <row r="247" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="64" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>